<commit_message>
Update template xm-web and hide unused variable
</commit_message>
<xml_diff>
--- a/Testcase Generate from Gitlab/input/Testcase-template-xm-web.xlsx
+++ b/Testcase Generate from Gitlab/input/Testcase-template-xm-web.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>Test Case Description</t>
   </si>
@@ -99,7 +99,10 @@
     <t>XM DEV website</t>
   </si>
   <si>
-    <t>Can login with ERP account, by user/ pass: superuser/ superuser</t>
+    <t>ERP user/ pass: superuser/ superuser</t>
+  </si>
+  <si>
+    <t>Can login with ERP account</t>
   </si>
 </sst>
 </file>
@@ -330,13 +333,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -402,12 +411,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -448,14 +451,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -467,34 +463,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -784,7 +752,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="D18" sqref="D18:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -795,50 +763,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="26"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="1">
         <v>43</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="17" t="s">
+      <c r="E1" s="28"/>
+      <c r="F1" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="16"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="26"/>
+      <c r="B2" s="28"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="30" t="s">
+      <c r="D2" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="26"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="28"/>
+      <c r="F2" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="26"/>
-      <c r="J2" s="34" t="s">
+      <c r="I2" s="28"/>
+      <c r="J2" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="35"/>
+      <c r="K2" s="37"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
@@ -854,10 +822,10 @@
       <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="37"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="10"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
@@ -882,31 +850,31 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="33" t="s">
+      <c r="D6" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="38">
+      <c r="E6" s="39"/>
+      <c r="F6" s="40">
         <f ca="1">TODAY()</f>
         <v>44999</v>
       </c>
-      <c r="G6" s="39"/>
-      <c r="H6" s="33" t="s">
+      <c r="G6" s="41"/>
+      <c r="H6" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="37"/>
-      <c r="J6" s="32" t="str">
+      <c r="I6" s="39"/>
+      <c r="J6" s="34" t="str">
         <f>IF(COUNTIF(I18:I34,"Fail")&gt;0, "Fail", "Pass")</f>
         <v>Pass</v>
       </c>
-      <c r="K6" s="32"/>
+      <c r="K6" s="34"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
@@ -925,88 +893,90 @@
       <c r="A8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
       <c r="E8" s="7"/>
       <c r="F8" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
     </row>
     <row r="9" spans="1:11" ht="13" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="3"/>
       <c r="F9" s="8">
         <v>1</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="16"/>
+      <c r="G9" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="18"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="8">
         <v>2</v>
       </c>
-      <c r="B10" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="20"/>
+      <c r="B10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="21"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="3"/>
       <c r="F10" s="8"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="19"/>
     </row>
     <row r="11" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8">
         <v>3</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="22"/>
       <c r="E11" s="3"/>
       <c r="F11" s="8"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
+      <c r="K11" s="19"/>
     </row>
     <row r="12" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="8">
         <v>4</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
       <c r="E12" s="3"/>
       <c r="F12" s="8"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="18"/>
+      <c r="K12" s="19"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
@@ -1037,79 +1007,79 @@
       <c r="K14" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="13" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="24" t="s">
+      <c r="C16" s="24"/>
+      <c r="D16" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E16" s="25"/>
-      <c r="F16" s="21" t="s">
+      <c r="E16" s="27"/>
+      <c r="F16" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="21" t="s">
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
     </row>
     <row r="18" spans="1:11" ht="25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>1</v>
       </c>
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="40" t="s">
+      <c r="C18" s="16"/>
+      <c r="D18" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E18" s="40"/>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="15"/>
+      <c r="F18" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="15" t="s">
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="16"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="19"/>
     </row>
     <row r="19" spans="1:11" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <f>A18+1</f>
         <v>2</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="40"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
       <c r="F19" s="42"/>
       <c r="G19" s="43"/>
       <c r="H19" s="44"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="16"/>
+      <c r="I19" s="17"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="19"/>
     </row>
     <row r="20" spans="1:11" s="14" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13">
@@ -1132,32 +1102,32 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B21" s="40"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="40"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
       <c r="F21" s="42"/>
       <c r="G21" s="43"/>
       <c r="H21" s="44"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" ht="17.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B22" s="40"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
       <c r="F22" s="42"/>
       <c r="G22" s="43"/>
       <c r="H22" s="44"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="16"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="49">
@@ -1212,15 +1182,15 @@
     <mergeCell ref="I18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="J6:K6">
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>J6="Fail"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="1" priority="5">
       <formula>J6="Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:K30">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$I18="Fail"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>